<commit_message>
Actualización 23 de julio 2023 - Lap HP
Se actualiza el repositorio con los materiales.
</commit_message>
<xml_diff>
--- a/Calificaciones de N02202315241 FISICA I_ 29_06_2023 21_05.xlsx
+++ b/Calificaciones de N02202315241 FISICA I_ 29_06_2023 21_05.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusto\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusto\OneDrive\Documentos\Cursos_UVM\Cuatrimestral\Fisica_1_BC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E40C33-0937-4F70-ADA8-70B45217E613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE95D683-0623-46B4-AD55-C2DCAF973AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <definedName name="Slicer_Assignments">#N/A</definedName>
     <definedName name="Slicer_Name">#N/A</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr/>
@@ -30,6 +30,17 @@
         <x14:slicerCache r:id="rId3"/>
         <x14:slicerCache r:id="rId4"/>
       </x15:slicerCaches>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -443,7 +454,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns="">
+      <mc:Fallback xmlns="" xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -521,7 +532,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns="">
+      <mc:Fallback xmlns="" xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name="Name"/>
@@ -5067,11 +5078,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E11C30F-3E38-423E-9165-B476CDC21D2A}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:B1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.5" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>